<commit_message>
Update before planned decom
</commit_message>
<xml_diff>
--- a/data/costs.xlsx
+++ b/data/costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\pypsa-za\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{234DF095-8292-491D-B3C4-4A3FC278906C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CBE505-28A0-4117-B9B3-C7795AF71104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="7840" windowWidth="18180" windowHeight="2820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="za_original" sheetId="5" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="155">
   <si>
     <t>technology</t>
   </si>
@@ -1640,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83FE029-657E-4ADB-BFF8-5DD15DBF8F4F}">
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:R94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B60" sqref="A60:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2146,7 +2146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>152</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>20</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>21</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2511,27 +2511,27 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <f>'[1]csir-today'!$C$2</f>
+        <f>'pypsa-za-original'!$C$3</f>
         <v>60447</v>
       </c>
       <c r="D28">
-        <f>'[1]csir-today'!$C$2</f>
+        <f>'pypsa-za-original'!$C$3</f>
         <v>60447</v>
       </c>
       <c r="E28">
-        <f>'[1]csir-today'!$C$2</f>
+        <f>'pypsa-za-original'!$C$3</f>
         <v>60447</v>
       </c>
       <c r="F28">
-        <f>'[1]csir-today'!$C$2</f>
+        <f>'pypsa-za-original'!$C$3</f>
         <v>60447</v>
       </c>
       <c r="G28">
-        <f>'[1]csir-today'!$C$2</f>
+        <f>'pypsa-za-original'!$C$3</f>
         <v>60447</v>
       </c>
       <c r="H28">
-        <f>'[1]csir-today'!$C$2</f>
+        <f>'pypsa-za-original'!$C$3</f>
         <v>60447</v>
       </c>
       <c r="I28" s="5" t="s">
@@ -2540,8 +2540,16 @@
       <c r="J28" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="Q28">
+        <f>C21/C28</f>
+        <v>0.58667923966449953</v>
+      </c>
+      <c r="R28">
+        <f>1-Q28</f>
+        <v>0.41332076033550047</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -2579,7 +2587,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>152</v>
       </c>
@@ -2616,7 +2624,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -2654,7 +2662,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -3365,28 +3373,22 @@
         <v>52</v>
       </c>
       <c r="C55">
-        <f>30*3.6</f>
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D55">
-        <f t="shared" ref="D55:H55" si="5">30*3.6</f>
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E55">
-        <f t="shared" si="5"/>
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="F55">
-        <f t="shared" si="5"/>
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G55">
-        <f t="shared" si="5"/>
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="H55">
-        <f t="shared" si="5"/>
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>151</v>
@@ -3407,23 +3409,23 @@
         <v>900</v>
       </c>
       <c r="D56">
-        <f t="shared" ref="D56:H56" si="6">50*18</f>
+        <f t="shared" ref="D56:H56" si="5">50*18</f>
         <v>900</v>
       </c>
       <c r="E56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
       <c r="F56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
       <c r="G56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
       <c r="H56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>900</v>
       </c>
       <c r="I56" s="5" t="s">
@@ -3860,24 +3862,19 @@
         <v>12000</v>
       </c>
       <c r="D70">
-        <f>0.9*C70</f>
-        <v>10800</v>
+        <v>12000</v>
       </c>
       <c r="E70">
-        <f t="shared" ref="E70:H70" si="7">0.9*D70</f>
-        <v>9720</v>
-      </c>
-      <c r="F70" s="6">
-        <f t="shared" si="7"/>
-        <v>8748</v>
+        <v>12000</v>
+      </c>
+      <c r="F70">
+        <v>12000</v>
       </c>
       <c r="G70">
-        <f t="shared" si="7"/>
-        <v>7873.2</v>
+        <v>12000</v>
       </c>
       <c r="H70">
-        <f t="shared" si="7"/>
-        <v>7085.88</v>
+        <v>12000</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>31</v>
@@ -6187,8 +6184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I102" sqref="I102"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection sqref="A1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6733,9 +6730,6 @@
       <c r="I18" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J18" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -6765,9 +6759,6 @@
       <c r="I19" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J19" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -6802,9 +6793,6 @@
       <c r="I20" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J20" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -6834,9 +6822,6 @@
       <c r="I21" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J21" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
@@ -6872,9 +6857,6 @@
       <c r="I22" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J22" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -6904,9 +6886,6 @@
       <c r="I23" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J23" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
@@ -6936,9 +6915,6 @@
       <c r="I24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J24" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -6968,9 +6944,6 @@
       <c r="I25" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J25" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
@@ -7000,9 +6973,6 @@
       <c r="I26" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J26" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -7032,9 +7002,6 @@
       <c r="I27" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J27" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -7064,9 +7031,6 @@
       <c r="I28" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J28" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
@@ -7096,9 +7060,6 @@
       <c r="I29" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J29" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
@@ -7133,9 +7094,6 @@
       <c r="I30" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J30" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
@@ -7912,25 +7870,25 @@
         <v>52</v>
       </c>
       <c r="C56">
-        <v>50</v>
+        <v>900</v>
       </c>
       <c r="D56">
-        <v>50</v>
+        <v>900</v>
       </c>
       <c r="E56">
-        <v>50</v>
+        <v>900</v>
       </c>
       <c r="F56">
-        <v>50</v>
+        <v>900</v>
       </c>
       <c r="G56">
-        <v>50</v>
+        <v>900</v>
       </c>
       <c r="H56">
-        <v>50</v>
+        <v>900</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="J56" t="s">
         <v>56</v>
@@ -8363,30 +8321,22 @@
         <v>12000</v>
       </c>
       <c r="D70">
-        <f>0.9*C70</f>
-        <v>10800</v>
+        <v>12000</v>
       </c>
       <c r="E70">
-        <f t="shared" ref="E70:H70" si="3">0.9*D70</f>
-        <v>9720</v>
+        <v>12000</v>
       </c>
       <c r="F70">
-        <f t="shared" si="3"/>
-        <v>8748</v>
+        <v>12000</v>
       </c>
       <c r="G70">
-        <f t="shared" si="3"/>
-        <v>7873.2</v>
+        <v>12000</v>
       </c>
       <c r="H70">
-        <f t="shared" si="3"/>
-        <v>7085.88</v>
+        <v>12000</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="J70" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
@@ -8513,9 +8463,6 @@
       <c r="I74" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="J74" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
@@ -8577,9 +8524,6 @@
       <c r="I76" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="J76" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
@@ -8673,9 +8617,6 @@
       <c r="I79" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="J79" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
@@ -8751,9 +8692,6 @@
       <c r="I82" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="J82" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
@@ -8829,9 +8767,6 @@
       <c r="I85" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="J85" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
@@ -8938,9 +8873,6 @@
       </c>
       <c r="I89" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="J89" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
@@ -9114,7 +9046,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="H3" sqref="G3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>